<commit_message>
language code for user form
next update table from form component
</commit_message>
<xml_diff>
--- a/Excel_sheets/language_component.xlsx
+++ b/Excel_sheets/language_component.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RIM_DEV\Core\rimdev\Excel_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2078BC-087F-4541-B1C2-6153A7D9B0EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
   <si>
     <t>type</t>
   </si>
@@ -120,12 +115,96 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>profile_img</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>idnumber</t>
+  </si>
+  <si>
+    <t>id_img</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>application_type</t>
+  </si>
+  <si>
+    <t>group_privil</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>ID_map</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>inserting_form</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>wrong_data</t>
+  </si>
+  <si>
+    <t>file_count_err</t>
+  </si>
+  <si>
+    <t>file_size_err</t>
+  </si>
+  <si>
+    <t>file_type_err</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>userpage</t>
+  </si>
+  <si>
+    <t>pages_use</t>
+  </si>
+  <si>
+    <t>created</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,211 +515,591 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>